<commit_message>
added details to pet creation
</commit_message>
<xml_diff>
--- a/Data/SaveFiles/Pets.xlsx
+++ b/Data/SaveFiles/Pets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -43,13 +43,22 @@
     <t>Owner</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
     <t>Draco</t>
   </si>
   <si>
-    <t>Dino</t>
+    <t>Dog🐶</t>
+  </si>
+  <si>
+    <t>Dino🦖</t>
   </si>
   <si>
     <t>05/30/2022</t>
+  </si>
+  <si>
+    <t>0 years, 0 months, and 0 days</t>
   </si>
   <si>
     <t>shy</t>
@@ -413,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,16 +465,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -474,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -482,28 +491,57 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="D4" t="s">
         <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addPets and viewPets complete
</commit_message>
<xml_diff>
--- a/Data/SaveFiles/Pets.xlsx
+++ b/Data/SaveFiles/Pets.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -43,46 +43,34 @@
     <t>ImageURL</t>
   </si>
   <si>
-    <t>tester</t>
-  </si>
-  <si>
-    <t>new</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>Cat🐱</t>
-  </si>
-  <si>
-    <t>Dog🐶</t>
-  </si>
-  <si>
-    <t>Pig🐷</t>
-  </si>
-  <si>
-    <t>Cow🐮</t>
+    <t>Draco</t>
+  </si>
+  <si>
+    <t>Tobee</t>
+  </si>
+  <si>
+    <t>Dino🦖</t>
+  </si>
+  <si>
+    <t>Bee🐝</t>
   </si>
   <si>
     <t>05/30/2022</t>
   </si>
   <si>
-    <t>0 years, 0 months, and 0 days</t>
-  </si>
-  <si>
-    <t>Mild</t>
-  </si>
-  <si>
-    <t>Naive</t>
-  </si>
-  <si>
-    <t>Brave</t>
-  </si>
-  <si>
-    <t>Jolly</t>
+    <t>0 y, 0 m, and 1 d</t>
+  </si>
+  <si>
+    <t>Hasty</t>
+  </si>
+  <si>
+    <t>Hardy</t>
   </si>
   <si>
     <t>Riccardo</t>
+  </si>
+  <si>
+    <t>Danni</t>
   </si>
 </sst>
 </file>
@@ -440,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,25 +471,25 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>22</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -509,85 +497,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
+      <c r="I3">
         <v>0</v>
       </c>
     </row>

</xml_diff>